<commit_message>
Added iso-risk curve graphs. Defined functions for percent balance increase/decrease with probabilities. Added cumulative distribution functions
Priming code for P-box integration.

Fixed first passage time for with/without potential recovery from bankruptcy.

Incoporated financial_balance into model. When below ROI threshold and financial balance of zero, classifies as bankruptcy.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -500,49 +500,49 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3701.045665800001</v>
+        <v>4112.272962000001</v>
       </c>
       <c r="D2" t="n">
-        <v>7562.872638810001</v>
+        <v>8403.191820900001</v>
       </c>
       <c r="E2" t="n">
-        <v>7706.91020841</v>
+        <v>8563.2335649</v>
       </c>
       <c r="F2" t="n">
-        <v>7810.437211560001</v>
+        <v>8678.263568400002</v>
       </c>
       <c r="G2" t="n">
-        <v>7905.862101420001</v>
+        <v>8784.291223800001</v>
       </c>
       <c r="H2" t="n">
-        <v>7993.184877990001</v>
+        <v>8881.316531100001</v>
       </c>
       <c r="I2" t="n">
-        <v>8074.206010890001</v>
+        <v>8971.340012100001</v>
       </c>
       <c r="J2" t="n">
-        <v>8130.020569110001</v>
+        <v>9033.356187900001</v>
       </c>
       <c r="K2" t="n">
-        <v>8182.234188090001</v>
+        <v>9091.371320100001</v>
       </c>
       <c r="L2" t="n">
-        <v>8231.747102640002</v>
+        <v>9146.3856696</v>
       </c>
       <c r="M2" t="n">
-        <v>8277.65907795</v>
+        <v>9197.3989755</v>
       </c>
       <c r="N2" t="n">
-        <v>8320.870348830002</v>
+        <v>9245.411498700001</v>
       </c>
       <c r="O2" t="n">
-        <v>8362.281150090001</v>
+        <v>9291.423500100002</v>
       </c>
       <c r="P2" t="n">
-        <v>8400.991246920001</v>
+        <v>9334.434718800001</v>
       </c>
       <c r="Q2" t="n">
-        <v>8437.000639320002</v>
+        <v>9374.445154800002</v>
       </c>
     </row>
     <row r="3">
@@ -555,49 +555,49 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>104.66513982</v>
+        <v>116.2945998</v>
       </c>
       <c r="D3" t="n">
-        <v>213.86156868</v>
+        <v>237.6239652</v>
       </c>
       <c r="E3" t="n">
-        <v>217.93463748</v>
+        <v>242.1495972</v>
       </c>
       <c r="F3" t="n">
-        <v>220.86215568</v>
+        <v>245.4023952</v>
       </c>
       <c r="G3" t="n">
-        <v>223.56056376</v>
+        <v>248.4006264</v>
       </c>
       <c r="H3" t="n">
-        <v>226.02986172</v>
+        <v>251.1442908</v>
       </c>
       <c r="I3" t="n">
-        <v>228.32096292</v>
+        <v>253.6899588</v>
       </c>
       <c r="J3" t="n">
-        <v>229.89927708</v>
+        <v>255.4436412</v>
       </c>
       <c r="K3" t="n">
-        <v>231.37576452</v>
+        <v>257.0841828</v>
       </c>
       <c r="L3" t="n">
-        <v>232.77588192</v>
+        <v>258.6398688</v>
       </c>
       <c r="M3" t="n">
-        <v>234.0741726</v>
+        <v>260.082414</v>
       </c>
       <c r="N3" t="n">
-        <v>235.29609324</v>
+        <v>261.4401036</v>
       </c>
       <c r="O3" t="n">
-        <v>236.46710052</v>
+        <v>262.7412228</v>
       </c>
       <c r="P3" t="n">
-        <v>237.56173776</v>
+        <v>263.9574864</v>
       </c>
       <c r="Q3" t="n">
-        <v>238.58000496</v>
+        <v>265.0888944</v>
       </c>
     </row>
     <row r="4">
@@ -610,49 +610,49 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>78.22909935</v>
+        <v>86.9212215</v>
       </c>
       <c r="D4" t="n">
-        <v>160.3961765100001</v>
+        <v>178.2179739000001</v>
       </c>
       <c r="E4" t="n">
-        <v>163.45097811</v>
+        <v>181.6121979</v>
       </c>
       <c r="F4" t="n">
-        <v>165.6466167600001</v>
+        <v>184.0517964</v>
       </c>
       <c r="G4" t="n">
-        <v>167.67042282</v>
+        <v>186.3004698</v>
       </c>
       <c r="H4" t="n">
-        <v>169.52239629</v>
+        <v>188.3582181</v>
       </c>
       <c r="I4" t="n">
-        <v>171.24072219</v>
+        <v>190.2674691</v>
       </c>
       <c r="J4" t="n">
-        <v>172.42445781</v>
+        <v>191.5827309</v>
       </c>
       <c r="K4" t="n">
-        <v>173.5318233900001</v>
+        <v>192.8131371</v>
       </c>
       <c r="L4" t="n">
-        <v>174.58191144</v>
+        <v>193.9799016</v>
       </c>
       <c r="M4" t="n">
-        <v>175.55562945</v>
+        <v>195.0618105</v>
       </c>
       <c r="N4" t="n">
-        <v>176.47206993</v>
+        <v>196.0800777</v>
       </c>
       <c r="O4" t="n">
-        <v>177.3503253900001</v>
+        <v>197.0559171</v>
       </c>
       <c r="P4" t="n">
-        <v>178.17130332</v>
+        <v>197.9681148000001</v>
       </c>
       <c r="Q4" t="n">
-        <v>178.9350037200001</v>
+        <v>198.8166708000001</v>
       </c>
     </row>
     <row r="5">
@@ -720,49 +720,49 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>114689.2547574</v>
+        <v>127432.505286</v>
       </c>
       <c r="D6" t="n">
-        <v>234371.3340681</v>
+        <v>260412.5934090001</v>
       </c>
       <c r="E6" t="n">
-        <v>238835.0185641</v>
+        <v>265372.242849</v>
       </c>
       <c r="F6" t="n">
-        <v>242043.2917956</v>
+        <v>268936.990884</v>
       </c>
       <c r="G6" t="n">
-        <v>245000.4827742</v>
+        <v>272222.758638</v>
       </c>
       <c r="H6" t="n">
-        <v>247706.5914999</v>
+        <v>275229.546111</v>
       </c>
       <c r="I6" t="n">
-        <v>250217.4140289</v>
+        <v>278019.348921</v>
       </c>
       <c r="J6" t="n">
-        <v>251947.0917711</v>
+        <v>279941.2130790001</v>
       </c>
       <c r="K6" t="n">
-        <v>253565.1774009001</v>
+        <v>281739.086001</v>
       </c>
       <c r="L6" t="n">
-        <v>255099.5689464</v>
+        <v>283443.965496</v>
       </c>
       <c r="M6" t="n">
-        <v>256522.3683795</v>
+        <v>285024.853755</v>
       </c>
       <c r="N6" t="n">
-        <v>257861.4737283</v>
+        <v>286512.748587</v>
       </c>
       <c r="O6" t="n">
-        <v>259144.7830209</v>
+        <v>287938.647801</v>
       </c>
       <c r="P6" t="n">
-        <v>260344.3982292</v>
+        <v>289271.553588</v>
       </c>
       <c r="Q6" t="n">
-        <v>261460.3193532001</v>
+        <v>290511.4659480001</v>
       </c>
     </row>
     <row r="7">
@@ -833,46 +833,46 @@
         <v>7200</v>
       </c>
       <c r="D8" t="n">
-        <v>7200</v>
+        <v>7920.000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>7200</v>
+        <v>8712.000000000002</v>
       </c>
       <c r="F8" t="n">
-        <v>7200</v>
+        <v>9583.200000000003</v>
       </c>
       <c r="G8" t="n">
-        <v>7200</v>
+        <v>10541.52</v>
       </c>
       <c r="H8" t="n">
-        <v>7200</v>
+        <v>11595.67200000001</v>
       </c>
       <c r="I8" t="n">
-        <v>7200</v>
+        <v>12755.23920000001</v>
       </c>
       <c r="J8" t="n">
-        <v>7200</v>
+        <v>14030.76312000001</v>
       </c>
       <c r="K8" t="n">
-        <v>7200</v>
+        <v>15433.83943200001</v>
       </c>
       <c r="L8" t="n">
-        <v>7200</v>
+        <v>16977.22337520001</v>
       </c>
       <c r="M8" t="n">
-        <v>7200</v>
+        <v>18674.94571272002</v>
       </c>
       <c r="N8" t="n">
-        <v>7200</v>
+        <v>20542.44028399202</v>
       </c>
       <c r="O8" t="n">
-        <v>7200</v>
+        <v>22596.68431239123</v>
       </c>
       <c r="P8" t="n">
-        <v>7200</v>
+        <v>24856.35274363035</v>
       </c>
       <c r="Q8" t="n">
-        <v>7200</v>
+        <v>27341.98801799339</v>
       </c>
     </row>
     <row r="9">
@@ -885,49 +885,49 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>1800</v>
+        <v>2400</v>
       </c>
       <c r="D9" t="n">
-        <v>1980</v>
+        <v>2760</v>
       </c>
       <c r="E9" t="n">
-        <v>2178</v>
+        <v>3174</v>
       </c>
       <c r="F9" t="n">
-        <v>2395.800000000001</v>
+        <v>3650.099999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>2635.380000000001</v>
+        <v>4197.614999999999</v>
       </c>
       <c r="H9" t="n">
-        <v>2898.918000000001</v>
+        <v>4827.257249999999</v>
       </c>
       <c r="I9" t="n">
-        <v>3188.809800000002</v>
+        <v>5551.345837499998</v>
       </c>
       <c r="J9" t="n">
-        <v>3507.690780000002</v>
+        <v>6384.047713124997</v>
       </c>
       <c r="K9" t="n">
-        <v>3858.459858000003</v>
+        <v>7341.654870093746</v>
       </c>
       <c r="L9" t="n">
-        <v>4244.305843800003</v>
+        <v>8442.903100607808</v>
       </c>
       <c r="M9" t="n">
-        <v>4668.736428180005</v>
+        <v>9709.338565698978</v>
       </c>
       <c r="N9" t="n">
-        <v>5135.610070998006</v>
+        <v>11165.73935055382</v>
       </c>
       <c r="O9" t="n">
-        <v>5649.171078097806</v>
+        <v>12840.6002531369</v>
       </c>
       <c r="P9" t="n">
-        <v>6214.088185907588</v>
+        <v>14766.69029110743</v>
       </c>
       <c r="Q9" t="n">
-        <v>6835.497004498347</v>
+        <v>16981.69383477354</v>
       </c>
     </row>
     <row r="10">
@@ -1050,49 +1050,49 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>213289.2547574</v>
+        <v>226632.505286</v>
       </c>
       <c r="D12" t="n">
-        <v>244151.3340681</v>
+        <v>271692.5934090001</v>
       </c>
       <c r="E12" t="n">
-        <v>248813.0185641</v>
+        <v>277858.242849</v>
       </c>
       <c r="F12" t="n">
-        <v>252239.0917956</v>
+        <v>282770.290884</v>
       </c>
       <c r="G12" t="n">
-        <v>255435.8627742</v>
+        <v>287561.893638</v>
       </c>
       <c r="H12" t="n">
-        <v>258405.5094999</v>
+        <v>292252.475361</v>
       </c>
       <c r="I12" t="n">
-        <v>261206.2238289</v>
+        <v>296925.9339585</v>
       </c>
       <c r="J12" t="n">
-        <v>263254.7825511</v>
+        <v>300956.0239121251</v>
       </c>
       <c r="K12" t="n">
-        <v>265223.6372589001</v>
+        <v>305114.5803030938</v>
       </c>
       <c r="L12" t="n">
-        <v>267143.8747902</v>
+        <v>309464.0919718078</v>
       </c>
       <c r="M12" t="n">
-        <v>268991.10480768</v>
+        <v>314009.138033419</v>
       </c>
       <c r="N12" t="n">
-        <v>270797.083799298</v>
+        <v>318820.9282215459</v>
       </c>
       <c r="O12" t="n">
-        <v>272593.9540989978</v>
+        <v>323975.9323665281</v>
       </c>
       <c r="P12" t="n">
-        <v>274358.4864151076</v>
+        <v>329494.5966227378</v>
       </c>
       <c r="Q12" t="n">
-        <v>276095.8163576984</v>
+        <v>335435.147800767</v>
       </c>
     </row>
     <row r="13">
@@ -1160,49 +1160,49 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>2867.231368935001</v>
+        <v>3185.812632150001</v>
       </c>
       <c r="D14" t="n">
-        <v>5859.283351702501</v>
+        <v>6510.314835225002</v>
       </c>
       <c r="E14" t="n">
-        <v>5970.8754641025</v>
+        <v>6634.306071225</v>
       </c>
       <c r="F14" t="n">
-        <v>6051.08229489</v>
+        <v>6723.424772100001</v>
       </c>
       <c r="G14" t="n">
-        <v>6125.012069355002</v>
+        <v>6805.56896595</v>
       </c>
       <c r="H14" t="n">
-        <v>6192.6647874975</v>
+        <v>6880.738652775</v>
       </c>
       <c r="I14" t="n">
-        <v>6255.435350722501</v>
+        <v>6950.483723025001</v>
       </c>
       <c r="J14" t="n">
-        <v>6298.677294277501</v>
+        <v>6998.530326975002</v>
       </c>
       <c r="K14" t="n">
-        <v>6339.129435022502</v>
+        <v>7043.477150025001</v>
       </c>
       <c r="L14" t="n">
-        <v>6377.489223660002</v>
+        <v>7086.0991374</v>
       </c>
       <c r="M14" t="n">
-        <v>6413.059209487499</v>
+        <v>7125.621343875</v>
       </c>
       <c r="N14" t="n">
-        <v>6446.536843207501</v>
+        <v>7162.818714675001</v>
       </c>
       <c r="O14" t="n">
-        <v>6478.619575522501</v>
+        <v>7198.466195025001</v>
       </c>
       <c r="P14" t="n">
-        <v>6508.609955730001</v>
+        <v>7231.788839700001</v>
       </c>
       <c r="Q14" t="n">
-        <v>6536.507983830002</v>
+        <v>7262.786648700003</v>
       </c>
     </row>
     <row r="15">
@@ -1215,49 +1215,49 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>41887.6363692</v>
+        <v>46541.818188</v>
       </c>
       <c r="D15" t="n">
-        <v>64206.69969487501</v>
+        <v>71340.77743875002</v>
       </c>
       <c r="E15" t="n">
-        <v>65429.538874875</v>
+        <v>72699.48763874998</v>
       </c>
       <c r="F15" t="n">
-        <v>66308.45453550002</v>
+        <v>73676.06059500002</v>
       </c>
       <c r="G15" t="n">
-        <v>67118.58549225</v>
+        <v>74576.2061025</v>
       </c>
       <c r="H15" t="n">
-        <v>67859.93174512501</v>
+        <v>75399.92416125</v>
       </c>
       <c r="I15" t="n">
-        <v>68547.77878387501</v>
+        <v>76164.19864875001</v>
       </c>
       <c r="J15" t="n">
-        <v>69021.62896612502</v>
+        <v>76690.69885125001</v>
       </c>
       <c r="K15" t="n">
-        <v>69464.908168875</v>
+        <v>77183.23129875</v>
       </c>
       <c r="L15" t="n">
-        <v>69885.25913700002</v>
+        <v>77650.28792999999</v>
       </c>
       <c r="M15" t="n">
-        <v>70275.03912562499</v>
+        <v>78083.37680625002</v>
       </c>
       <c r="N15" t="n">
-        <v>70641.890879625</v>
+        <v>78490.98986625001</v>
       </c>
       <c r="O15" t="n">
-        <v>70993.457143875</v>
+        <v>78881.61904875001</v>
       </c>
       <c r="P15" t="n">
-        <v>71322.0951735</v>
+        <v>79246.772415</v>
       </c>
       <c r="Q15" t="n">
-        <v>71627.80496850002</v>
+        <v>79586.44996500001</v>
       </c>
     </row>
     <row r="16">
@@ -1270,49 +1270,49 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1220.073603513402</v>
+        <v>1355.637337237114</v>
       </c>
       <c r="D16" t="n">
-        <v>2493.365865689691</v>
+        <v>2770.40651743299</v>
       </c>
       <c r="E16" t="n">
-        <v>2540.852895627835</v>
+        <v>2823.169884030928</v>
       </c>
       <c r="F16" t="n">
-        <v>2574.984198395877</v>
+        <v>2861.093553773197</v>
       </c>
       <c r="G16" t="n">
-        <v>2606.444355729897</v>
+        <v>2896.04928414433</v>
       </c>
       <c r="H16" t="n">
-        <v>2635.233367629897</v>
+        <v>2928.03707514433</v>
       </c>
       <c r="I16" t="n">
-        <v>2661.944821970103</v>
+        <v>2957.71646885567</v>
       </c>
       <c r="J16" t="n">
-        <v>2680.346046071134</v>
+        <v>2978.162273412371</v>
       </c>
       <c r="K16" t="n">
-        <v>2697.560094423712</v>
+        <v>2997.288993804124</v>
       </c>
       <c r="L16" t="n">
-        <v>2713.883760964949</v>
+        <v>3015.426401072165</v>
       </c>
       <c r="M16" t="n">
-        <v>2729.020251757732</v>
+        <v>3032.244724175258</v>
       </c>
       <c r="N16" t="n">
-        <v>2743.266360739176</v>
+        <v>3048.073734154639</v>
       </c>
       <c r="O16" t="n">
-        <v>2756.918881846392</v>
+        <v>3063.243202051547</v>
       </c>
       <c r="P16" t="n">
-        <v>2769.681021142268</v>
+        <v>3077.423356824743</v>
       </c>
       <c r="Q16" t="n">
-        <v>2781.552778626805</v>
+        <v>3090.614198474228</v>
       </c>
     </row>
     <row r="17">
@@ -1435,49 +1435,49 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>69325.46811064841</v>
+        <v>74433.79492638713</v>
       </c>
       <c r="D19" t="n">
-        <v>103911.2408502672</v>
+        <v>111973.390729408</v>
       </c>
       <c r="E19" t="n">
-        <v>105293.1591726053</v>
+        <v>113508.8555320059</v>
       </c>
       <c r="F19" t="n">
-        <v>106286.4129667859</v>
+        <v>114612.4708588732</v>
       </c>
       <c r="G19" t="n">
-        <v>107201.9338553349</v>
+        <v>115629.7162905943</v>
       </c>
       <c r="H19" t="n">
-        <v>108039.7218382524</v>
+        <v>116560.5918271693</v>
       </c>
       <c r="I19" t="n">
-        <v>108817.0508945676</v>
+        <v>117424.2907786307</v>
       </c>
       <c r="J19" t="n">
-        <v>109352.5442444737</v>
+        <v>118019.2833896374</v>
       </c>
       <c r="K19" t="n">
-        <v>109853.4896363212</v>
+        <v>118575.8893805791</v>
       </c>
       <c r="L19" t="n">
-        <v>110328.524059625</v>
+        <v>119103.7054064722</v>
       </c>
       <c r="M19" t="n">
-        <v>110769.0105248702</v>
+        <v>119593.1348123003</v>
       </c>
       <c r="N19" t="n">
-        <v>111183.5860215717</v>
+        <v>120053.7742530796</v>
       </c>
       <c r="O19" t="n">
-        <v>111580.8875392439</v>
+        <v>120495.2203838266</v>
       </c>
       <c r="P19" t="n">
-        <v>111952.2780883723</v>
+        <v>120907.8765495247</v>
       </c>
       <c r="Q19" t="n">
-        <v>112297.7576689568</v>
+        <v>121291.7427501742</v>
       </c>
     </row>
     <row r="20">
@@ -1490,49 +1490,49 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>143963.7866467516</v>
+        <v>152198.7103596129</v>
       </c>
       <c r="D20" t="n">
-        <v>140240.0932178328</v>
+        <v>159719.2026795921</v>
       </c>
       <c r="E20" t="n">
-        <v>143519.8593914947</v>
+        <v>164349.3873169941</v>
       </c>
       <c r="F20" t="n">
-        <v>145952.6788288141</v>
+        <v>168157.8200251268</v>
       </c>
       <c r="G20" t="n">
-        <v>148233.9289188652</v>
+        <v>171932.1773474057</v>
       </c>
       <c r="H20" t="n">
-        <v>150365.7876616476</v>
+        <v>175691.8835338307</v>
       </c>
       <c r="I20" t="n">
-        <v>152389.1729343324</v>
+        <v>179501.6431798694</v>
       </c>
       <c r="J20" t="n">
-        <v>153902.2383066264</v>
+        <v>182936.7405224877</v>
       </c>
       <c r="K20" t="n">
-        <v>155370.1476225789</v>
+        <v>186538.6909225147</v>
       </c>
       <c r="L20" t="n">
-        <v>156815.3507305751</v>
+        <v>190360.3865653356</v>
       </c>
       <c r="M20" t="n">
-        <v>158222.0942828098</v>
+        <v>194416.0032211188</v>
       </c>
       <c r="N20" t="n">
-        <v>159613.4977777264</v>
+        <v>198767.1539684662</v>
       </c>
       <c r="O20" t="n">
-        <v>161013.0665597539</v>
+        <v>203480.7119827016</v>
       </c>
       <c r="P20" t="n">
-        <v>162406.2083267354</v>
+        <v>208586.720073213</v>
       </c>
       <c r="Q20" t="n">
-        <v>163798.0586887416</v>
+        <v>214143.4050505928</v>
       </c>
     </row>
     <row r="21">
@@ -1603,46 +1603,46 @@
         <v>60750</v>
       </c>
       <c r="D22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="E22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="F22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="G22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="H22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="I22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="J22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="K22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="L22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="M22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="N22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="O22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="P22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
       <c r="Q22" t="n">
-        <v>81378</v>
+        <v>105678</v>
       </c>
     </row>
     <row r="23">
@@ -1658,46 +1658,46 @@
         <v>4860</v>
       </c>
       <c r="D23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="E23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="F23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="G23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="H23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="I23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="J23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="K23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="L23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="M23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="N23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="O23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="P23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
       <c r="Q23" t="n">
-        <v>6510.24</v>
+        <v>8454.24</v>
       </c>
     </row>
     <row r="24">
@@ -1823,46 +1823,46 @@
         <v>75210</v>
       </c>
       <c r="D26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="E26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="F26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="G26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="H26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="I26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="J26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="K26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="L26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="M26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="N26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="O26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="P26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
       <c r="Q26" t="n">
-        <v>114288.24</v>
+        <v>140532.24</v>
       </c>
     </row>
     <row r="27">
@@ -1875,49 +1875,49 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>68753.78664675163</v>
+        <v>76988.71035961289</v>
       </c>
       <c r="D27" t="n">
-        <v>25951.85321783282</v>
+        <v>19186.96267959208</v>
       </c>
       <c r="E27" t="n">
-        <v>29231.61939149465</v>
+        <v>23817.14731699409</v>
       </c>
       <c r="F27" t="n">
-        <v>31664.43882881409</v>
+        <v>27625.58002512681</v>
       </c>
       <c r="G27" t="n">
-        <v>33945.68891886515</v>
+        <v>31399.93734740571</v>
       </c>
       <c r="H27" t="n">
-        <v>36077.54766164756</v>
+        <v>35159.64353383071</v>
       </c>
       <c r="I27" t="n">
-        <v>38100.93293433239</v>
+        <v>38969.40317986938</v>
       </c>
       <c r="J27" t="n">
-        <v>39613.99830662635</v>
+        <v>42404.50052248774</v>
       </c>
       <c r="K27" t="n">
-        <v>41081.90762257889</v>
+        <v>46006.45092251466</v>
       </c>
       <c r="L27" t="n">
-        <v>42527.11073057506</v>
+        <v>49828.14656533563</v>
       </c>
       <c r="M27" t="n">
-        <v>43933.85428280979</v>
+        <v>53883.76322111877</v>
       </c>
       <c r="N27" t="n">
-        <v>45325.25777772635</v>
+        <v>58234.91396846625</v>
       </c>
       <c r="O27" t="n">
-        <v>46724.8265597539</v>
+        <v>62948.47198270159</v>
       </c>
       <c r="P27" t="n">
-        <v>48117.96832673535</v>
+        <v>68054.48007321302</v>
       </c>
       <c r="Q27" t="n">
-        <v>49509.81868874158</v>
+        <v>73611.1650505928</v>
       </c>
     </row>
     <row r="28">
@@ -2150,49 +2150,49 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>30554.7675331542</v>
+        <v>38789.69124601546</v>
       </c>
       <c r="D32" t="n">
-        <v>-21956.05708352957</v>
+        <v>-28720.9476217703</v>
       </c>
       <c r="E32" t="n">
-        <v>-18676.29090986773</v>
+        <v>-24090.7629843683</v>
       </c>
       <c r="F32" t="n">
-        <v>-16243.47147254829</v>
+        <v>-20282.33027623557</v>
       </c>
       <c r="G32" t="n">
-        <v>-13962.22138249723</v>
+        <v>-16507.97295395668</v>
       </c>
       <c r="H32" t="n">
-        <v>16659.76528611766</v>
+        <v>15741.86115830081</v>
       </c>
       <c r="I32" t="n">
-        <v>18683.15055880249</v>
+        <v>19551.62080433948</v>
       </c>
       <c r="J32" t="n">
-        <v>20196.21593109645</v>
+        <v>22986.71814695784</v>
       </c>
       <c r="K32" t="n">
-        <v>21664.12524704899</v>
+        <v>26588.66854698476</v>
       </c>
       <c r="L32" t="n">
-        <v>23109.32835504516</v>
+        <v>30410.36418980573</v>
       </c>
       <c r="M32" t="n">
-        <v>24516.07190727989</v>
+        <v>34465.98084558887</v>
       </c>
       <c r="N32" t="n">
-        <v>25907.47540219645</v>
+        <v>38817.13159293635</v>
       </c>
       <c r="O32" t="n">
-        <v>27307.044184224</v>
+        <v>43530.68960717169</v>
       </c>
       <c r="P32" t="n">
-        <v>28700.18595120545</v>
+        <v>48636.69769768312</v>
       </c>
       <c r="Q32" t="n">
-        <v>30092.03631321168</v>
+        <v>54193.38267506289</v>
       </c>
     </row>
     <row r="33">
@@ -2205,49 +2205,49 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>13.69507957181281</v>
+        <v>17.38608901552959</v>
       </c>
       <c r="D33" t="n">
-        <v>-9.841015760173292</v>
+        <v>-12.87313551416203</v>
       </c>
       <c r="E33" t="n">
-        <v>-8.370978108062181</v>
+        <v>-10.79782117990632</v>
       </c>
       <c r="F33" t="n">
-        <v>-7.280553978937633</v>
+        <v>-9.090827699259538</v>
       </c>
       <c r="G33" t="n">
-        <v>-6.258065378016201</v>
+        <v>-7.399107289180288</v>
       </c>
       <c r="H33" t="n">
-        <v>7.467142762370522</v>
+        <v>7.055725131517756</v>
       </c>
       <c r="I33" t="n">
-        <v>8.374052699871601</v>
+        <v>8.763313364528113</v>
       </c>
       <c r="J33" t="n">
-        <v>9.05223003008483</v>
+        <v>10.30297264660365</v>
       </c>
       <c r="K33" t="n">
-        <v>9.710167776276545</v>
+        <v>11.91741783223847</v>
       </c>
       <c r="L33" t="n">
-        <v>10.3579282784621</v>
+        <v>13.63035594806253</v>
       </c>
       <c r="M33" t="n">
-        <v>10.98845066303219</v>
+        <v>15.44814077504419</v>
       </c>
       <c r="N33" t="n">
-        <v>11.61209741664287</v>
+        <v>17.39838816767179</v>
       </c>
       <c r="O33" t="n">
-        <v>12.23940396758601</v>
+        <v>19.51107163028576</v>
       </c>
       <c r="P33" t="n">
-        <v>12.86382983935626</v>
+        <v>21.7996567755662</v>
       </c>
       <c r="Q33" t="n">
-        <v>13.48767688512575</v>
+        <v>24.29024168471793</v>
       </c>
     </row>
     <row r="34">
@@ -2257,52 +2257,52 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-3553.815269689905</v>
+        <v>6446.184730310095</v>
       </c>
       <c r="C34" t="n">
-        <v>-84552.86300622561</v>
+        <v>-66317.93929336435</v>
       </c>
       <c r="D34" t="n">
-        <v>-106508.9200897552</v>
+        <v>-95038.88691513466</v>
       </c>
       <c r="E34" t="n">
-        <v>-125185.2109996229</v>
+        <v>-119129.649899503</v>
       </c>
       <c r="F34" t="n">
-        <v>-141428.6824721712</v>
+        <v>-139411.9801757385</v>
       </c>
       <c r="G34" t="n">
-        <v>-155390.9038546684</v>
+        <v>-155919.9531296952</v>
       </c>
       <c r="H34" t="n">
-        <v>-138731.1385685508</v>
+        <v>-140178.0919713944</v>
       </c>
       <c r="I34" t="n">
-        <v>-120047.9880097483</v>
+        <v>-120626.4711670549</v>
       </c>
       <c r="J34" t="n">
-        <v>-99851.77207865182</v>
+        <v>-97639.75302009709</v>
       </c>
       <c r="K34" t="n">
-        <v>-78187.64683160283</v>
+        <v>-71051.08447311234</v>
       </c>
       <c r="L34" t="n">
-        <v>-55078.31847655767</v>
+        <v>-40640.72028330661</v>
       </c>
       <c r="M34" t="n">
-        <v>-30562.24656927779</v>
+        <v>-6174.739437717741</v>
       </c>
       <c r="N34" t="n">
-        <v>-4654.771167081337</v>
+        <v>32642.39215521861</v>
       </c>
       <c r="O34" t="n">
-        <v>22652.27301714266</v>
+        <v>76173.0817623903</v>
       </c>
       <c r="P34" t="n">
-        <v>51352.45896834812</v>
+        <v>124809.7794600734</v>
       </c>
       <c r="Q34" t="n">
-        <v>81444.49528155979</v>
+        <v>179003.1621351363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>